<commit_message>
Add new resequencing to abundance calculations
</commit_message>
<xml_diff>
--- a/scripts_figures_and_tables/relative_abundance/tables/characteristic_abundances_strain1.xlsx
+++ b/scripts_figures_and_tables/relative_abundance/tables/characteristic_abundances_strain1.xlsx
@@ -385,7 +385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,7 +393,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:31">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -463,8 +463,29 @@
       <c r="X1" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:31">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,70 +496,91 @@
         <v>0.4795918367346939</v>
       </c>
       <c r="D2" t="n">
+        <v>0.5567010309278351</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.6703296703296704</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
+        <v>0.6994818652849741</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.7411764705882353</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.5652173913043478</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0.4693877551020407</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
+        <v>0.5789473684210527</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.5402298850574713</v>
       </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>0.5491329479768786</v>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>0.4470046082949309</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>0.4619883040935673</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
         <v>0.468599033816425</v>
       </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
         <v>0.4380952380952381</v>
       </c>
-      <c r="N2" t="n">
+      <c r="Q2" t="n">
         <v>0.53</v>
       </c>
-      <c r="O2" t="n">
+      <c r="R2" t="n">
         <v>0.4672131147540983</v>
       </c>
-      <c r="P2" t="n">
+      <c r="S2" t="n">
         <v>0.5124378109452737</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="T2" t="n">
+        <v>0.4764397905759162</v>
+      </c>
+      <c r="U2" t="n">
         <v>0.6157635467980295</v>
       </c>
-      <c r="R2" t="n">
+      <c r="V2" t="n">
         <v>0.6972972972972973</v>
       </c>
-      <c r="S2" t="n">
+      <c r="W2" t="n">
+        <v>0.663551401869159</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.6393442622950819</v>
+      </c>
+      <c r="Y2" t="n">
         <v>0.5436893203883496</v>
       </c>
-      <c r="T2" t="n">
+      <c r="Z2" t="n">
+        <v>0.592039800995025</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.4975369458128078</v>
       </c>
-      <c r="U2" t="n">
+      <c r="AB2" t="n">
         <v>0.5376344086021506</v>
       </c>
-      <c r="V2" t="n">
+      <c r="AC2" t="n">
         <v>0.5752212389380531</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AD2" t="n">
         <v>0.5692307692307692</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AE2" t="n">
         <v>0.4956521739130436</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:31">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -549,70 +591,91 @@
         <v>0.5204081632653061</v>
       </c>
       <c r="D3" t="n">
+        <v>0.4432989690721649</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.3296703296703297</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
+        <v>0.3005181347150259</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.2588235294117647</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.4347826086956522</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.5306122448979592</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
+        <v>0.4210526315789473</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.4597701149425288</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.4508670520231214</v>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>0.5529953917050692</v>
       </c>
-      <c r="K3" t="n">
+      <c r="N3" t="n">
         <v>0.5380116959064328</v>
       </c>
-      <c r="L3" t="n">
+      <c r="O3" t="n">
         <v>0.5314009661835748</v>
       </c>
-      <c r="M3" t="n">
+      <c r="P3" t="n">
         <v>0.561904761904762</v>
       </c>
-      <c r="N3" t="n">
+      <c r="Q3" t="n">
         <v>0.47</v>
       </c>
-      <c r="O3" t="n">
+      <c r="R3" t="n">
         <v>0.5327868852459016</v>
       </c>
-      <c r="P3" t="n">
+      <c r="S3" t="n">
         <v>0.4875621890547264</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="T3" t="n">
+        <v>0.5235602094240838</v>
+      </c>
+      <c r="U3" t="n">
         <v>0.3842364532019704</v>
       </c>
-      <c r="R3" t="n">
+      <c r="V3" t="n">
         <v>0.3027027027027027</v>
       </c>
-      <c r="S3" t="n">
+      <c r="W3" t="n">
+        <v>0.3364485981308412</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.360655737704918</v>
+      </c>
+      <c r="Y3" t="n">
         <v>0.4563106796116504</v>
       </c>
-      <c r="T3" t="n">
+      <c r="Z3" t="n">
+        <v>0.4079601990049752</v>
+      </c>
+      <c r="AA3" t="n">
         <v>0.5024630541871921</v>
       </c>
-      <c r="U3" t="n">
+      <c r="AB3" t="n">
         <v>0.4623655913978495</v>
       </c>
-      <c r="V3" t="n">
+      <c r="AC3" t="n">
         <v>0.424778761061947</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AD3" t="n">
         <v>0.4307692307692308</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AE3" t="n">
         <v>0.5043478260869565</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:31">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -647,38 +710,49 @@
         <v>0.5026737967914439</v>
       </c>
       <c r="L4" t="n">
+        <v>0.5167464114832536</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.4908256880733945</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>0.5863636363636363</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>0.4687500000000001</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>0.6284153005464481</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>0.4423963133640553</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>0.6382978723404256</v>
       </c>
-      <c r="R4" t="n">
+      <c r="T4" t="n">
         <v>0.6553398058252428</v>
       </c>
-      <c r="S4" t="n">
+      <c r="U4" t="n">
         <v>0.5497630331753555</v>
       </c>
-      <c r="T4" t="n">
+      <c r="V4" t="n">
         <v>0.6380952380952382</v>
       </c>
-      <c r="U4" t="s"/>
-      <c r="V4" t="s"/>
       <c r="W4" t="s"/>
       <c r="X4" t="s"/>
+      <c r="Y4" t="s"/>
+      <c r="Z4" t="s"/>
+      <c r="AA4" t="s"/>
+      <c r="AB4" t="s"/>
+      <c r="AC4" t="s"/>
+      <c r="AD4" t="s"/>
+      <c r="AE4" t="s"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:31">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -713,38 +787,49 @@
         <v>0.4973262032085561</v>
       </c>
       <c r="L5" t="n">
+        <v>0.4832535885167464</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.5091743119266056</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.4545454545454545</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>0.4136363636363636</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>0.53125</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>0.3715846994535519</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>0.5576036866359447</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="S5" t="n">
         <v>0.3617021276595744</v>
       </c>
-      <c r="R5" t="n">
+      <c r="T5" t="n">
         <v>0.3446601941747572</v>
       </c>
-      <c r="S5" t="n">
+      <c r="U5" t="n">
         <v>0.4502369668246445</v>
       </c>
-      <c r="T5" t="n">
+      <c r="V5" t="n">
         <v>0.3619047619047619</v>
       </c>
-      <c r="U5" t="s"/>
-      <c r="V5" t="s"/>
       <c r="W5" t="s"/>
       <c r="X5" t="s"/>
+      <c r="Y5" t="s"/>
+      <c r="Z5" t="s"/>
+      <c r="AA5" t="s"/>
+      <c r="AB5" t="s"/>
+      <c r="AC5" t="s"/>
+      <c r="AD5" t="s"/>
+      <c r="AE5" t="s"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:31">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -776,39 +861,48 @@
         <v>0.3059360730593607</v>
       </c>
       <c r="K6" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.1380952380952381</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.1369047619047619</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>0.1931150293870697</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>0.4044444444444444</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>0.2157598499061914</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.1723804925156929</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>0.1146401985111662</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>0.2307692307692308</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>0.1317671092951992</v>
       </c>
-      <c r="T6" t="s"/>
       <c r="U6" t="s"/>
       <c r="V6" t="s"/>
       <c r="W6" t="s"/>
       <c r="X6" t="s"/>
+      <c r="Y6" t="s"/>
+      <c r="Z6" t="s"/>
+      <c r="AA6" t="s"/>
+      <c r="AB6" t="s"/>
+      <c r="AC6" t="s"/>
+      <c r="AD6" t="s"/>
+      <c r="AE6" t="s"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:31">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -840,37 +934,46 @@
         <v>0.6940639269406393</v>
       </c>
       <c r="K7" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.8619047619047618</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.8630952380952381</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>0.8068849706129303</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>0.5955555555555556</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>0.7842401500938085</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>0.8276195074843072</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>0.8853598014888338</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>0.7692307692307693</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>0.8682328907048008</v>
       </c>
-      <c r="T7" t="s"/>
       <c r="U7" t="s"/>
       <c r="V7" t="s"/>
       <c r="W7" t="s"/>
       <c r="X7" t="s"/>
+      <c r="Y7" t="s"/>
+      <c r="Z7" t="s"/>
+      <c r="AA7" t="s"/>
+      <c r="AB7" t="s"/>
+      <c r="AC7" t="s"/>
+      <c r="AD7" t="s"/>
+      <c r="AE7" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>